<commit_message>
Sending appliance category and capacity in vendor invoices minor bug fix: All invoice type not working other minor changes
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Vendor_Settlement_Template-Cash-v3.xlsx
+++ b/application/controllers/excel-templates/Vendor_Settlement_Template-Cash-v3.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>Blackmelon Advance Technology Co. Pvt. Ltd.</t>
   </si>
@@ -198,6 +198,18 @@
   </si>
   <si>
     <t xml:space="preserve">247around Royalty %    </t>
+  </si>
+  <si>
+    <t>Appliance Category</t>
+  </si>
+  <si>
+    <t>Appliance Capacity</t>
+  </si>
+  <si>
+    <t>{booking:appliance_category}</t>
+  </si>
+  <si>
+    <t>{booking:appliance_capacity}</t>
   </si>
 </sst>
 </file>
@@ -756,7 +768,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -921,12 +933,69 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1009,51 +1078,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1074,13 +1098,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>290287</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>136072</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>319318</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>150911</xdr:rowOff>
@@ -1406,26 +1430,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="E11" sqref="E11:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="1" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.5" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="8.5" customWidth="1"/>
-    <col min="11" max="11" width="7.6640625" customWidth="1"/>
-    <col min="12" max="12" width="5.83203125" customWidth="1"/>
+    <col min="7" max="7" width="9.5" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
+    <col min="12" max="12" width="8.5" customWidth="1"/>
+    <col min="13" max="13" width="7.6640625" customWidth="1"/>
+    <col min="14" max="14" width="5.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1438,124 +1462,140 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" ht="14" x14ac:dyDescent="0.2">
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="22" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25" t="s">
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="5"/>
-    </row>
-    <row r="3" spans="1:12" ht="14" x14ac:dyDescent="0.2">
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="26" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="29" t="s">
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="8"/>
-    </row>
-    <row r="4" spans="1:12" ht="14" x14ac:dyDescent="0.2">
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="26" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="29" t="s">
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="8"/>
-    </row>
-    <row r="5" spans="1:12" ht="14" x14ac:dyDescent="0.2">
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="8"/>
+    </row>
+    <row r="5" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="26" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
       <c r="G5" s="28"/>
       <c r="H5" s="28"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="8"/>
-    </row>
-    <row r="6" spans="1:12" ht="14" x14ac:dyDescent="0.2">
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="8"/>
+    </row>
+    <row r="6" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="26" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="28"/>
       <c r="H6" s="28"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" ht="14" x14ac:dyDescent="0.2">
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="8"/>
+    </row>
+    <row r="7" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="26" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="27"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
       <c r="K7" s="6"/>
-      <c r="L7" s="8"/>
-    </row>
-    <row r="8" spans="1:12" ht="14" x14ac:dyDescent="0.2">
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="8"/>
+    </row>
+    <row r="8" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="30"/>
       <c r="C8" s="31"/>
       <c r="D8" s="31"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
       <c r="G8" s="28"/>
       <c r="H8" s="28"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="8"/>
-    </row>
-    <row r="9" spans="1:12" ht="14" x14ac:dyDescent="0.2">
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="8"/>
+    </row>
+    <row r="9" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="32" t="s">
         <v>3</v>
@@ -1564,32 +1604,36 @@
       <c r="D9" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="28"/>
       <c r="H9" s="28"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="8"/>
-    </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="8"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="34"/>
       <c r="C10" s="35"/>
       <c r="D10" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
       <c r="G10" s="36"/>
       <c r="H10" s="36"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="11"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
       <c r="K10" s="12"/>
-      <c r="L10" s="13"/>
-    </row>
-    <row r="11" spans="1:12" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L10" s="11"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="13"/>
+    </row>
+    <row r="11" spans="1:14" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="18" t="s">
         <v>4</v>
@@ -1600,32 +1644,38 @@
       <c r="D11" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="H11" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="I11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="J11" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="20" t="s">
+      <c r="K11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="L11" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="K11" s="20" t="s">
+      <c r="M11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="L11" s="21" t="s">
+      <c r="N11" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="15" t="s">
         <v>17</v>
@@ -1637,31 +1687,37 @@
         <v>19</v>
       </c>
       <c r="E12" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="H12" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="I12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="J12" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="K12" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="L12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="K12" s="16" t="s">
+      <c r="M12" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="17" t="s">
+      <c r="N12" s="17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="14" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="14"/>
       <c r="C13" s="6"/>
@@ -1673,312 +1729,344 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="8"/>
-    </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="8"/>
+    </row>
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="63"/>
-      <c r="L14" s="64"/>
-    </row>
-    <row r="15" spans="1:12" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="82"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="82"/>
+      <c r="K14" s="82"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="82"/>
+      <c r="N14" s="83"/>
+    </row>
+    <row r="15" spans="1:14" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="61"/>
-    </row>
-    <row r="16" spans="1:12" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="80"/>
+    </row>
+    <row r="16" spans="1:14" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="38" t="s">
+      <c r="B16" s="77"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="39" t="s">
+      <c r="J16" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="I16" s="39" t="s">
+      <c r="K16" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="J16" s="39" t="s">
+      <c r="L16" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="K16" s="39" t="s">
+      <c r="M16" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="L16" s="40" t="s">
+      <c r="N16" s="40" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
-      <c r="B17" s="83"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="84"/>
-      <c r="F17" s="85"/>
-      <c r="G17" s="41" t="s">
+      <c r="B17" s="102"/>
+      <c r="C17" s="103"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="103"/>
+      <c r="F17" s="103"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="104"/>
+      <c r="I17" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42" t="s">
+      <c r="J17" s="42"/>
+      <c r="K17" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="J17" s="43" t="s">
+      <c r="L17" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="K17" s="43" t="s">
+      <c r="M17" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="L17" s="44" t="s">
+      <c r="N17" s="44" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
-      <c r="B18" s="80" t="s">
+      <c r="B18" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="81"/>
-      <c r="D18" s="81"/>
-      <c r="E18" s="81"/>
-      <c r="F18" s="82"/>
-      <c r="G18" s="45">
+      <c r="C18" s="100"/>
+      <c r="D18" s="100"/>
+      <c r="E18" s="100"/>
+      <c r="F18" s="100"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="101"/>
+      <c r="I18" s="45">
         <v>0.3</v>
       </c>
-      <c r="H18" s="46"/>
-      <c r="I18" s="47">
+      <c r="J18" s="46"/>
+      <c r="K18" s="47">
         <v>0.15</v>
       </c>
-      <c r="J18" s="48">
+      <c r="L18" s="48">
         <v>0.05</v>
       </c>
-      <c r="K18" s="49"/>
-      <c r="L18" s="50"/>
-    </row>
-    <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M18" s="49"/>
+      <c r="N18" s="50"/>
+    </row>
+    <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
-      <c r="B19" s="80" t="s">
+      <c r="B19" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="81"/>
-      <c r="F19" s="82"/>
-      <c r="G19" s="41" t="s">
+      <c r="C19" s="100"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="100"/>
+      <c r="F19" s="100"/>
+      <c r="G19" s="100"/>
+      <c r="H19" s="101"/>
+      <c r="I19" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="H19" s="42"/>
-      <c r="I19" s="51" t="s">
+      <c r="J19" s="42"/>
+      <c r="K19" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="J19" s="49" t="s">
+      <c r="L19" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="K19" s="49"/>
-      <c r="L19" s="50"/>
-    </row>
-    <row r="20" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M19" s="49"/>
+      <c r="N19" s="50"/>
+    </row>
+    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
-      <c r="B20" s="80" t="s">
+      <c r="B20" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="81"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="93" t="s">
+      <c r="C20" s="100"/>
+      <c r="D20" s="100"/>
+      <c r="E20" s="100"/>
+      <c r="F20" s="100"/>
+      <c r="G20" s="100"/>
+      <c r="H20" s="101"/>
+      <c r="I20" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="H20" s="92"/>
-      <c r="I20" s="92"/>
-      <c r="J20" s="92"/>
-      <c r="K20" s="92"/>
-      <c r="L20" s="94"/>
-    </row>
-    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="67"/>
+      <c r="M20" s="67"/>
+      <c r="N20" s="68"/>
+    </row>
+    <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="53"/>
       <c r="C21" s="54"/>
       <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="98"/>
-      <c r="H21" s="99"/>
-      <c r="I21" s="99"/>
-      <c r="J21" s="99"/>
-      <c r="K21" s="99"/>
-      <c r="L21" s="100"/>
-    </row>
-    <row r="22" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="70"/>
+      <c r="L21" s="70"/>
+      <c r="M21" s="70"/>
+      <c r="N21" s="71"/>
+    </row>
+    <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
-      <c r="B22" s="89" t="s">
+      <c r="B22" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="90"/>
-      <c r="D22" s="90"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="91"/>
-      <c r="G22" s="95" t="s">
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="H22" s="96"/>
-      <c r="I22" s="96"/>
-      <c r="J22" s="96"/>
-      <c r="K22" s="96"/>
-      <c r="L22" s="97"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="52"/>
-    </row>
-    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J22" s="73"/>
+      <c r="K22" s="73"/>
+      <c r="L22" s="73"/>
+      <c r="M22" s="73"/>
+      <c r="N22" s="74"/>
+      <c r="O22" s="52"/>
+      <c r="P22" s="52"/>
+    </row>
+    <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
-      <c r="B23" s="86"/>
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="87"/>
-      <c r="J23" s="87"/>
-      <c r="K23" s="87"/>
-      <c r="L23" s="88"/>
-    </row>
-    <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="60"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="61"/>
+      <c r="K23" s="61"/>
+      <c r="L23" s="61"/>
+      <c r="M23" s="61"/>
+      <c r="N23" s="62"/>
+    </row>
+    <row r="24" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
-      <c r="B24" s="65" t="s">
+      <c r="B24" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="78"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="78"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="78"/>
-      <c r="K24" s="78"/>
-      <c r="L24" s="79"/>
-    </row>
-    <row r="25" spans="1:14" ht="14" x14ac:dyDescent="0.2">
+      <c r="C24" s="97"/>
+      <c r="D24" s="97"/>
+      <c r="E24" s="97"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="97"/>
+      <c r="H24" s="97"/>
+      <c r="I24" s="97"/>
+      <c r="J24" s="97"/>
+      <c r="K24" s="97"/>
+      <c r="L24" s="97"/>
+      <c r="M24" s="97"/>
+      <c r="N24" s="98"/>
+    </row>
+    <row r="25" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="76" t="s">
+      <c r="C25" s="76"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="57"/>
-      <c r="L25" s="77"/>
-    </row>
-    <row r="26" spans="1:14" ht="14" x14ac:dyDescent="0.2">
+      <c r="H25" s="76"/>
+      <c r="I25" s="76"/>
+      <c r="J25" s="76"/>
+      <c r="K25" s="76"/>
+      <c r="L25" s="76"/>
+      <c r="M25" s="76"/>
+      <c r="N25" s="96"/>
+    </row>
+    <row r="26" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
-      <c r="B26" s="67" t="s">
+      <c r="B26" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="68"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="73">
+      <c r="C26" s="87"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="92">
         <v>102405500277</v>
       </c>
-      <c r="F26" s="74"/>
-      <c r="G26" s="74"/>
-      <c r="H26" s="74"/>
-      <c r="I26" s="74"/>
-      <c r="J26" s="74"/>
-      <c r="K26" s="74"/>
-      <c r="L26" s="75"/>
-    </row>
-    <row r="27" spans="1:14" ht="14" x14ac:dyDescent="0.2">
+      <c r="H26" s="93"/>
+      <c r="I26" s="93"/>
+      <c r="J26" s="93"/>
+      <c r="K26" s="93"/>
+      <c r="L26" s="93"/>
+      <c r="M26" s="93"/>
+      <c r="N26" s="94"/>
+    </row>
+    <row r="27" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
-      <c r="B27" s="67" t="s">
+      <c r="B27" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="68"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="71" t="s">
+      <c r="C27" s="87"/>
+      <c r="D27" s="87"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="68"/>
-      <c r="L27" s="72"/>
-    </row>
-    <row r="28" spans="1:14" ht="14" x14ac:dyDescent="0.2">
+      <c r="H27" s="87"/>
+      <c r="I27" s="87"/>
+      <c r="J27" s="87"/>
+      <c r="K27" s="87"/>
+      <c r="L27" s="87"/>
+      <c r="M27" s="87"/>
+      <c r="N27" s="91"/>
+    </row>
+    <row r="28" spans="1:16" ht="14" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
-      <c r="B28" s="65" t="s">
+      <c r="B28" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="66"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="69" t="s">
+      <c r="C28" s="85"/>
+      <c r="D28" s="85"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="66"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="66"/>
-      <c r="J28" s="66"/>
-      <c r="K28" s="66"/>
-      <c r="L28" s="70"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="85"/>
+      <c r="J28" s="85"/>
+      <c r="K28" s="85"/>
+      <c r="L28" s="85"/>
+      <c r="M28" s="85"/>
+      <c r="N28" s="89"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="21">
-    <mergeCell ref="B23:L23"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="G20:L20"/>
-    <mergeCell ref="G21:L21"/>
-    <mergeCell ref="G22:L22"/>
     <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B15:L15"/>
-    <mergeCell ref="B14:L14"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B15:N15"/>
+    <mergeCell ref="B14:N14"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E28:L28"/>
-    <mergeCell ref="E27:L27"/>
-    <mergeCell ref="E26:L26"/>
-    <mergeCell ref="E25:L25"/>
-    <mergeCell ref="B24:L24"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="G28:N28"/>
+    <mergeCell ref="G27:N27"/>
+    <mergeCell ref="G26:N26"/>
+    <mergeCell ref="G25:N25"/>
+    <mergeCell ref="B24:N24"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B23:N23"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="I20:N20"/>
+    <mergeCell ref="I21:N21"/>
+    <mergeCell ref="I22:N22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>